<commit_message>
Removed print messages, updated comments, updated Excel results.
</commit_message>
<xml_diff>
--- a/result_analysis.xlsx
+++ b/result_analysis.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="17">
   <si>
     <t>Problem</t>
   </si>
@@ -56,13 +56,28 @@
     <t>Time</t>
   </si>
   <si>
-    <t>not solved</t>
-  </si>
-  <si>
     <t>4. Depth first limited search</t>
   </si>
   <si>
     <t>5. Uniform cost search</t>
+  </si>
+  <si>
+    <t>6. Recursive best first search H1</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>8.</t>
+  </si>
+  <si>
+    <t>9. astar_search h_ignore_preconditions</t>
+  </si>
+  <si>
+    <t>10.</t>
+  </si>
+  <si>
+    <t>not solved within 10min timeframe</t>
   </si>
 </sst>
 </file>
@@ -78,12 +93,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -377,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -423,7 +445,7 @@
       <c r="D3">
         <v>180</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>6</v>
       </c>
       <c r="F3">
@@ -443,7 +465,7 @@
       <c r="D4">
         <v>30509</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>9</v>
       </c>
       <c r="F4">
@@ -463,7 +485,7 @@
       <c r="D5">
         <v>129631</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>12</v>
       </c>
       <c r="F5">
@@ -508,7 +530,7 @@
       <c r="D9">
         <v>5960</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>6</v>
       </c>
       <c r="F9">
@@ -520,7 +542,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -528,7 +550,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -618,7 +640,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -666,7 +688,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -674,12 +696,12 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -715,7 +737,7 @@
       <c r="D27">
         <v>224</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <v>6</v>
       </c>
       <c r="F27">
@@ -735,7 +757,7 @@
       <c r="D28">
         <v>44030</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>9</v>
       </c>
       <c r="F28">
@@ -755,11 +777,271 @@
       <c r="D29">
         <v>159716</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <v>12</v>
       </c>
       <c r="F29">
         <v>57.43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>4229</v>
+      </c>
+      <c r="C33">
+        <v>4330</v>
+      </c>
+      <c r="D33">
+        <v>17023</v>
+      </c>
+      <c r="E33" s="1">
+        <v>6</v>
+      </c>
+      <c r="F33">
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>41</v>
+      </c>
+      <c r="C51">
+        <v>43</v>
+      </c>
+      <c r="D51">
+        <v>170</v>
+      </c>
+      <c r="E51" s="1">
+        <v>6</v>
+      </c>
+      <c r="F51">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52">
+        <v>1450</v>
+      </c>
+      <c r="C52">
+        <v>1452</v>
+      </c>
+      <c r="D52">
+        <v>13303</v>
+      </c>
+      <c r="E52" s="1">
+        <v>9</v>
+      </c>
+      <c r="F52">
+        <v>3.82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>5040</v>
+      </c>
+      <c r="C53">
+        <v>5042</v>
+      </c>
+      <c r="D53">
+        <v>44944</v>
+      </c>
+      <c r="E53" s="1">
+        <v>12</v>
+      </c>
+      <c r="F53">
+        <v>16.350000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean up code. Integrate results into Excel and Word.
</commit_message>
<xml_diff>
--- a/result_analysis.xlsx
+++ b/result_analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="41480" yWindow="-14860" windowWidth="21480" windowHeight="20200" tabRatio="500"/>
+    <workbookView xWindow="4120" yWindow="460" windowWidth="21480" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -498,15 +498,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -516,12 +513,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -539,6 +530,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -826,7 +826,7 @@
   <dimension ref="A2:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -835,30 +835,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="32" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
@@ -881,7 +881,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -902,7 +902,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="13">
         <v>3</v>
       </c>
@@ -923,7 +923,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3">
@@ -946,33 +946,33 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="7">
         <v>2</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="24"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="9">
         <v>3</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="25"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="3">
@@ -987,7 +987,7 @@
       <c r="E9" s="4">
         <v>84</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="20">
         <v>20</v>
       </c>
       <c r="G9" s="6">
@@ -995,7 +995,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="7">
         <v>2</v>
       </c>
@@ -1008,7 +1008,7 @@
       <c r="E10" s="1">
         <v>5602</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="21">
         <v>619</v>
       </c>
       <c r="G10" s="8">
@@ -1016,7 +1016,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="9">
         <v>3</v>
       </c>
@@ -1029,7 +1029,7 @@
       <c r="E11" s="10">
         <v>3364</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="22">
         <v>392</v>
       </c>
       <c r="G11" s="12">
@@ -1037,7 +1037,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="3">
@@ -1052,7 +1052,7 @@
       <c r="E12" s="4">
         <v>414</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="20">
         <v>50</v>
       </c>
       <c r="G12" s="6">
@@ -1060,33 +1060,33 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="7">
         <v>2</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="24"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="9">
         <v>3</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="25"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="19"/>
       <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="3">
@@ -1109,7 +1109,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="7">
         <v>2</v>
       </c>
@@ -1130,7 +1130,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="9">
         <v>3</v>
       </c>
@@ -1151,7 +1151,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="3">
@@ -1174,33 +1174,33 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="7">
         <v>2</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="24"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="18"/>
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="9">
         <v>3</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="25"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="19"/>
       <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="3">
@@ -1223,7 +1223,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="7">
         <v>2</v>
       </c>
@@ -1236,7 +1236,7 @@
       <c r="E22" s="1">
         <v>8910</v>
       </c>
-      <c r="F22" s="27">
+      <c r="F22" s="21">
         <v>17</v>
       </c>
       <c r="G22" s="8">
@@ -1244,7 +1244,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="9">
         <v>3</v>
       </c>
@@ -1257,7 +1257,7 @@
       <c r="E23" s="10">
         <v>49429</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="22">
         <v>22</v>
       </c>
       <c r="G23" s="12">
@@ -1265,7 +1265,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="3">
@@ -1288,7 +1288,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="7">
         <v>2</v>
       </c>
@@ -1309,7 +1309,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="9">
         <v>3</v>
       </c>
@@ -1330,7 +1330,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="3">
@@ -1353,7 +1353,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="7">
         <v>2</v>
       </c>
@@ -1374,7 +1374,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="9">
         <v>3</v>
       </c>
@@ -1395,42 +1395,77 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="6"/>
+      <c r="C30" s="4">
+        <v>11</v>
+      </c>
+      <c r="D30" s="4">
+        <v>13</v>
+      </c>
+      <c r="E30" s="4">
+        <v>50</v>
+      </c>
+      <c r="F30" s="5">
+        <v>6</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0.56000000000000005</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="21"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="7">
         <v>2</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="8"/>
+      <c r="C31" s="1">
+        <v>86</v>
+      </c>
+      <c r="D31" s="1">
+        <v>88</v>
+      </c>
+      <c r="E31" s="1">
+        <v>841</v>
+      </c>
+      <c r="F31" s="2">
+        <v>9</v>
+      </c>
+      <c r="G31" s="8">
+        <v>45.1</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="9">
         <v>3</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="12"/>
+      <c r="C32" s="10">
+        <v>318</v>
+      </c>
+      <c r="D32" s="10">
+        <v>320</v>
+      </c>
+      <c r="E32" s="10">
+        <v>2934</v>
+      </c>
+      <c r="F32" s="11">
+        <v>12</v>
+      </c>
+      <c r="G32" s="12">
+        <v>228.64</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A27:A29"/>
@@ -1441,11 +1476,6 @@
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="C20:E20"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>